<commit_message>
fix: Vm licenses - Subscription Usage
</commit_message>
<xml_diff>
--- a/clouds_labs/lab2-Azure/Azure lab team 8.xlsx
+++ b/clouds_labs/lab2-Azure/Azure lab team 8.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="147">
   <si>
     <t>IT Tower</t>
   </si>
@@ -280,10 +280,13 @@
     <t>Licensing</t>
   </si>
   <si>
+    <t>Subscription Usage</t>
+  </si>
+  <si>
+    <t>Red Hat Enterprise Linux</t>
+  </si>
+  <si>
     <t>Compute Hours</t>
-  </si>
-  <si>
-    <t>Red Hat Enterprise Linux</t>
   </si>
   <si>
     <t>Red Hat Enterprise Linux%</t>
@@ -1136,19 +1139,19 @@
         <v>90</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>86</v>
       </c>
       <c r="G17" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="H17" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="H17" s="2" t="s">
-        <v>89</v>
-      </c>
       <c r="I17" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="18">
@@ -1162,19 +1165,19 @@
         <v>86</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>86</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
     </row>
     <row r="19">
@@ -1188,22 +1191,22 @@
         <v>86</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="F19" s="2" t="s">
         <v>86</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="20">
@@ -1217,22 +1220,22 @@
         <v>86</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="F20" s="2" t="s">
         <v>86</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="21">
@@ -1246,22 +1249,22 @@
         <v>86</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="F21" s="2" t="s">
         <v>86</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="22">
@@ -1275,22 +1278,22 @@
         <v>86</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="F22" s="2" t="s">
         <v>86</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="23">
@@ -1298,25 +1301,25 @@
         <v>16</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D23" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="F23" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="E23" s="2" t="s">
+      <c r="G23" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="F23" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="G23" s="2" t="s">
-        <v>105</v>
-      </c>
       <c r="H23" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="24">
@@ -1324,25 +1327,25 @@
         <v>16</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="E24" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="G24" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="F24" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="G24" s="2" t="s">
-        <v>108</v>
-      </c>
       <c r="H24" s="2" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="25">
@@ -1350,25 +1353,25 @@
         <v>16</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="26">
@@ -1376,25 +1379,25 @@
         <v>16</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D26" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="E26" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="E26" s="2" t="s">
-        <v>112</v>
-      </c>
       <c r="F26" s="2" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="27">
@@ -1405,25 +1408,25 @@
         <v>47</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D27" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="F27" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="E27" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="F27" s="2" t="s">
-        <v>115</v>
-      </c>
       <c r="G27" s="2" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="28">
@@ -1434,22 +1437,22 @@
         <v>47</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D28" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="I28" s="2" t="s">
         <v>121</v>
-      </c>
-      <c r="E28" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="F28" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="H28" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="I28" s="2" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="29">
@@ -1460,25 +1463,25 @@
         <v>47</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="30">
@@ -1492,19 +1495,19 @@
         <v>59</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="F30" s="2" t="s">
         <v>62</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="I30" s="2" t="s">
         <v>65</v>
@@ -1518,25 +1521,25 @@
         <v>58</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>60</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="I31" s="2" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="32">
@@ -1550,22 +1553,22 @@
         <v>59</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="I32" s="2" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="33">
@@ -1579,19 +1582,19 @@
         <v>59</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="I33" s="2" t="s">
         <v>65</v>
@@ -1608,13 +1611,13 @@
         <v>59</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="35">
@@ -1625,16 +1628,21 @@
         <v>47</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="D35" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="F35" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="E35" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="F35" s="2" t="s">
-        <v>143</v>
+    </row>
+    <row r="39">
+      <c r="E39" s="2" t="s">
+        <v>89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>